<commit_message>
update Payment Notice Document
</commit_message>
<xml_diff>
--- a/IG-Publisher/output/StructureDefinition-PaymentNoticeDocument.xlsx
+++ b/IG-Publisher/output/StructureDefinition-PaymentNoticeDocument.xlsx
@@ -361,7 +361,7 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -401,32 +401,28 @@
     <t>Composition.status</t>
   </si>
   <si>
-    <t>preliminary | final | amended | entered-in-error</t>
-  </si>
-  <si>
-    <t>The workflow/clinical status of this composition. The status is a marker for the clinical standing of the document.</t>
-  </si>
-  <si>
-    <t>If a composition is marked as withdrawn, the compositions/documents in the series, or data from the composition or document series, should never be displayed to a user without being clearly marked as untrustworthy. The flag "entered-in-error" is why this element is labeled as a modifier of other elements.   
-Some reporting work flows require that the original narrative of a final document never be altered; instead, only new narrative can be added. The composition resource has no explicit status for explicitly noting whether this business rule is in effect. This would be handled by an extension if required.</t>
-  </si>
-  <si>
-    <t>Need to be able to mark interim, amended, or withdrawn compositions or documents.</t>
+    <t>active | cancelled | draft | entered-in-error</t>
+  </si>
+  <si>
+    <t>The status of the resource instance.</t>
+  </si>
+  <si>
+    <t>This element is labeled as a modifier because the status contains codes that mark the resource as not currently valid.</t>
+  </si>
+  <si>
+    <t>Need to track the status of the resource as 'draft' resources may undergo further edits while 'active' resources are immutable and may only have their status changed to 'cancelled'.</t>
   </si>
   <si>
     <t>required</t>
   </si>
   <si>
-    <t>The workflow/clinical status of the composition.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/composition-status|4.0.1</t>
+    <t>A code specifying the state of the resource instance.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/fm-status|4.0.1</t>
   </si>
   <si>
     <t>Event.status</t>
-  </si>
-  <si>
-    <t>interim: .completionCode="IN" &amp; ./statusCode[isNormalDatatype()]="active";  final: .completionCode="AU" &amp;&amp;  ./statusCode[isNormalDatatype()]="complete" and not(./inboundRelationship[typeCode="SUBJ" and isNormalActRelationship()]/source[subsumesCode("ActClass#CACT") and moodCode="EVN" and domainMember("ReviseComposition", code) and isNormalAct()]);  amended: .completionCode="AU" &amp;&amp;  ./statusCode[isNormalDatatype()]="complete" and ./inboundRelationship[typeCode="SUBJ" and isNormalActRelationship()]/source[subsumesCode("ActClass#CACT") and moodCode="EVN" and domainMember("ReviseComposition", code) and isNormalAct() and statusCode="completed"];  withdrawn : .completionCode=NI &amp;&amp;  ./statusCode[isNormalDatatype()]="obsolete"</t>
   </si>
   <si>
     <t>FiveWs.status</t>
@@ -741,6 +737,9 @@
   <si>
     <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>BackboneElement.modifierExtension</t>
@@ -1414,7 +1413,7 @@
     <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="26.71484375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="249.5078125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="32.84375" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="52.33203125" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="25.01171875" customWidth="true" bestFit="true"/>
@@ -2854,10 +2853,10 @@
         <v>130</v>
       </c>
       <c r="AK12" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AL12" t="s" s="2">
         <v>131</v>
-      </c>
-      <c r="AL12" t="s" s="2">
-        <v>132</v>
       </c>
       <c r="AM12" t="s" s="2">
         <v>43</v>
@@ -2869,12 +2868,12 @@
         <v>51</v>
       </c>
       <c r="AP12" t="s" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2897,19 +2896,19 @@
         <v>56</v>
       </c>
       <c r="J13" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="K13" t="s" s="2">
         <v>135</v>
       </c>
-      <c r="K13" t="s" s="2">
+      <c r="L13" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="L13" t="s" s="2">
+      <c r="M13" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="M13" t="s" s="2">
+      <c r="N13" t="s" s="2">
         <v>138</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>139</v>
       </c>
       <c r="O13" t="s" s="2">
         <v>43</v>
@@ -2937,11 +2936,11 @@
         <v>79</v>
       </c>
       <c r="X13" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="Y13" t="s" s="2">
         <v>140</v>
       </c>
-      <c r="Y13" t="s" s="2">
-        <v>141</v>
-      </c>
       <c r="Z13" t="s" s="2">
         <v>43</v>
       </c>
@@ -2958,7 +2957,7 @@
         <v>43</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>55</v>
@@ -2973,30 +2972,30 @@
         <v>67</v>
       </c>
       <c r="AJ13" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="AK13" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="AK13" t="s" s="2">
+      <c r="AL13" t="s" s="2">
         <v>143</v>
       </c>
-      <c r="AL13" t="s" s="2">
+      <c r="AM13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO13" t="s" s="2">
         <v>144</v>
       </c>
-      <c r="AM13" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN13" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO13" t="s" s="2">
+      <c r="AP13" t="s" s="2">
         <v>145</v>
-      </c>
-      <c r="AP13" t="s" s="2">
-        <v>146</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -3019,19 +3018,19 @@
         <v>56</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L14" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="L14" t="s" s="2">
+      <c r="M14" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="M14" t="s" s="2">
+      <c r="N14" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>151</v>
       </c>
       <c r="O14" t="s" s="2">
         <v>43</v>
@@ -3056,14 +3055,14 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="X14" t="s" s="2">
         <v>152</v>
       </c>
-      <c r="X14" t="s" s="2">
+      <c r="Y14" t="s" s="2">
         <v>153</v>
       </c>
-      <c r="Y14" t="s" s="2">
-        <v>154</v>
-      </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>44</v>
@@ -3095,13 +3094,13 @@
         <v>67</v>
       </c>
       <c r="AJ14" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AK14" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="AK14" t="s" s="2">
-        <v>156</v>
-      </c>
       <c r="AL14" t="s" s="2">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AM14" t="s" s="2">
         <v>43</v>
@@ -3113,12 +3112,12 @@
         <v>51</v>
       </c>
       <c r="AP14" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3141,19 +3140,19 @@
         <v>56</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="L15" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>161</v>
       </c>
-      <c r="M15" t="s" s="2">
+      <c r="N15" t="s" s="2">
         <v>162</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>163</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>43</v>
@@ -3202,7 +3201,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>44</v>
@@ -3220,27 +3219,27 @@
         <v>43</v>
       </c>
       <c r="AK15" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="AL15" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="AL15" t="s" s="2">
+      <c r="AM15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN15" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO15" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="AM15" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN15" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO15" t="s" s="2">
+      <c r="AP15" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="AP15" t="s" s="2">
-        <v>167</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3263,17 +3262,17 @@
         <v>56</v>
       </c>
       <c r="J16" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K16" t="s" s="2">
         <v>169</v>
       </c>
-      <c r="K16" t="s" s="2">
+      <c r="L16" t="s" s="2">
         <v>170</v>
-      </c>
-      <c r="L16" t="s" s="2">
-        <v>171</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>43</v>
@@ -3322,7 +3321,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>44</v>
@@ -3337,30 +3336,30 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="AL16" t="s" s="2">
+      <c r="AM16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO16" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="AM16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN16" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO16" t="s" s="2">
+      <c r="AP16" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="AP16" t="s" s="2">
-        <v>177</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3383,19 +3382,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>181</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>182</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>183</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>43</v>
@@ -3444,7 +3443,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>55</v>
@@ -3459,30 +3458,30 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>184</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AL17" t="s" s="2">
         <v>185</v>
       </c>
-      <c r="AL17" t="s" s="2">
+      <c r="AM17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN17" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO17" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="AM17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN17" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO17" t="s" s="2">
+      <c r="AP17" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="AP17" t="s" s="2">
-        <v>188</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3505,17 +3504,17 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>192</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>43</v>
@@ -3564,7 +3563,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>55</v>
@@ -3579,30 +3578,30 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="AK18" t="s" s="2">
         <v>194</v>
       </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AL18" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="AL18" t="s" s="2">
+      <c r="AM18" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN18" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO18" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="AM18" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN18" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO18" t="s" s="2">
+      <c r="AP18" t="s" s="2">
         <v>197</v>
-      </c>
-      <c r="AP18" t="s" s="2">
-        <v>198</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3628,13 +3627,13 @@
         <v>57</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>201</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>202</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3684,7 +3683,7 @@
         <v>43</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>55</v>
@@ -3702,27 +3701,27 @@
         <v>43</v>
       </c>
       <c r="AK19" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM19" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN19" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO19" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="AL19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO19" t="s" s="2">
+      <c r="AP19" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AP19" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3748,13 +3747,13 @@
         <v>75</v>
       </c>
       <c r="K20" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>207</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>209</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3783,11 +3782,11 @@
         <v>127</v>
       </c>
       <c r="X20" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="Y20" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="Y20" t="s" s="2">
-        <v>211</v>
-      </c>
       <c r="Z20" t="s" s="2">
         <v>43</v>
       </c>
@@ -3804,7 +3803,7 @@
         <v>43</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>44</v>
@@ -3822,27 +3821,27 @@
         <v>43</v>
       </c>
       <c r="AK20" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM20" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN20" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO20" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AP20" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM20" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN20" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO20" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="AP20" t="s" s="2">
-        <v>213</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3865,19 +3864,19 @@
         <v>43</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="K21" t="s" s="2">
         <v>215</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="L21" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>43</v>
@@ -3926,7 +3925,7 @@
         <v>43</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>44</v>
@@ -3944,27 +3943,27 @@
         <v>43</v>
       </c>
       <c r="AK21" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AL21" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM21" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN21" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO21" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="AL21" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM21" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO21" t="s" s="2">
+      <c r="AP21" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="AP21" t="s" s="2">
-        <v>222</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3990,10 +3989,10 @@
         <v>57</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>225</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -4044,7 +4043,7 @@
         <v>43</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>44</v>
@@ -4082,7 +4081,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4111,7 +4110,7 @@
         <v>102</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M23" t="s" s="2">
         <v>104</v>
@@ -4164,7 +4163,7 @@
         <v>43</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>44</v>
@@ -4202,11 +4201,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4228,16 +4227,16 @@
         <v>101</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="M24" t="s" s="2">
         <v>104</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>43</v>
@@ -4467,7 +4466,7 @@
         <v>43</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K26" t="s" s="2">
         <v>244</v>
@@ -4829,7 +4828,7 @@
         <v>43</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K29" t="s" s="2">
         <v>267</v>
@@ -4952,10 +4951,10 @@
         <v>57</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>225</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -5006,7 +5005,7 @@
         <v>43</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>44</v>
@@ -5073,7 +5072,7 @@
         <v>102</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M31" t="s" s="2">
         <v>104</v>
@@ -5126,7 +5125,7 @@
         <v>43</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>44</v>
@@ -5168,7 +5167,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -5190,16 +5189,16 @@
         <v>101</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>104</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>43</v>
@@ -5547,7 +5546,7 @@
         <v>56</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K35" t="s" s="2">
         <v>293</v>
@@ -5672,10 +5671,10 @@
         <v>57</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>225</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5726,7 +5725,7 @@
         <v>43</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>44</v>
@@ -5793,7 +5792,7 @@
         <v>102</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M37" t="s" s="2">
         <v>104</v>
@@ -5846,7 +5845,7 @@
         <v>43</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>44</v>
@@ -5888,7 +5887,7 @@
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
@@ -5910,16 +5909,16 @@
         <v>101</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="M38" t="s" s="2">
         <v>104</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>43</v>
@@ -6029,7 +6028,7 @@
         <v>56</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K39" t="s" s="2">
         <v>304</v>
@@ -6064,7 +6063,7 @@
         <v>43</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="X39" t="s" s="2">
         <v>307</v>
@@ -6106,7 +6105,7 @@
         <v>43</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>43</v>
@@ -6118,7 +6117,7 @@
         <v>43</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AP39" t="s" s="2">
         <v>309</v>
@@ -6224,7 +6223,7 @@
         <v>43</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>43</v>
@@ -6236,7 +6235,7 @@
         <v>43</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AP40" t="s" s="2">
         <v>314</v>
@@ -6267,7 +6266,7 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K41" t="s" s="2">
         <v>316</v>
@@ -6385,7 +6384,7 @@
         <v>43</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K42" t="s" s="2">
         <v>320</v>
@@ -6506,10 +6505,10 @@
         <v>57</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>225</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6560,7 +6559,7 @@
         <v>43</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>44</v>
@@ -6627,7 +6626,7 @@
         <v>102</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M44" t="s" s="2">
         <v>104</v>
@@ -6680,7 +6679,7 @@
         <v>43</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>44</v>
@@ -6722,7 +6721,7 @@
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
@@ -6744,16 +6743,16 @@
         <v>101</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>43</v>
@@ -6942,19 +6941,19 @@
         <v>43</v>
       </c>
       <c r="AK46" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM46" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN46" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO46" t="s" s="2">
         <v>203</v>
-      </c>
-      <c r="AL46" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN46" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO46" t="s" s="2">
-        <v>204</v>
       </c>
       <c r="AP46" t="s" s="2">
         <v>43</v>
@@ -6985,7 +6984,7 @@
         <v>43</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K47" t="s" s="2">
         <v>335</v>
@@ -7022,7 +7021,7 @@
         <v>43</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="X47" t="s" s="2">
         <v>339</v>
@@ -7064,7 +7063,7 @@
         <v>43</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>43</v>
@@ -7076,7 +7075,7 @@
         <v>43</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AP47" t="s" s="2">
         <v>43</v>
@@ -7107,7 +7106,7 @@
         <v>43</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K48" t="s" s="2">
         <v>342</v>
@@ -7117,7 +7116,7 @@
       </c>
       <c r="M48" s="2"/>
       <c r="N48" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>43</v>
@@ -7184,19 +7183,19 @@
         <v>43</v>
       </c>
       <c r="AK48" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="AL48" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="AL48" t="s" s="2">
+      <c r="AM48" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>197</v>
       </c>
       <c r="AP48" t="s" s="2">
         <v>43</v>
@@ -7227,7 +7226,7 @@
         <v>43</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K49" t="s" s="2">
         <v>345</v>
@@ -7549,7 +7548,7 @@
         <v>362</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>43</v>
@@ -7589,7 +7588,7 @@
         <v>43</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K52" t="s" s="2">
         <v>364</v>
@@ -7711,7 +7710,7 @@
         <v>43</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K53" t="s" s="2">
         <v>372</v>
@@ -7831,7 +7830,7 @@
         <v>43</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K54" t="s" s="2">
         <v>379</v>

</xml_diff>